<commit_message>
Updated for SEC scraping rules
</commit_message>
<xml_diff>
--- a/Filing Names/Default Filing Terms.xlsx
+++ b/Filing Names/Default Filing Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\Desktop\Work\Quant_project\Scrape_Code\Filing Names\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D598119D-25AB-426B-9011-71C4A2F94178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363C5770-726A-4875-9E97-A53D68E2AB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D13A5E3-946E-45B2-A307-58457D115325}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Consolidated Balance Sheet</t>
   </si>
@@ -73,12 +73,6 @@
     <t>Consolidated Statements of Operations and Comprehensive Income (Loss)</t>
   </si>
   <si>
-    <t>Consolidated Statements of Cash Flows</t>
-  </si>
-  <si>
-    <t>Consolidated Statements of Stockholder's (Deficit) Equity</t>
-  </si>
-  <si>
     <t>cash and cash equivalents</t>
   </si>
   <si>
@@ -196,12 +190,6 @@
     <t>retained earnings</t>
   </si>
   <si>
-    <t>common stock</t>
-  </si>
-  <si>
-    <t>treasury stock</t>
-  </si>
-  <si>
     <t>accumulated deficit</t>
   </si>
   <si>
@@ -229,42 +217,12 @@
     <t>operating income</t>
   </si>
   <si>
-    <t>common stock repurchased</t>
-  </si>
-  <si>
     <t>income statement</t>
   </si>
   <si>
     <t>balance sheet</t>
   </si>
   <si>
-    <t>cash flow from operations</t>
-  </si>
-  <si>
-    <t>net cash from operations</t>
-  </si>
-  <si>
-    <t>cash flow from investing</t>
-  </si>
-  <si>
-    <t>statements of stockholders equity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treasury shares </t>
-  </si>
-  <si>
-    <t>common stock issued</t>
-  </si>
-  <si>
-    <t>stock-compensation expense</t>
-  </si>
-  <si>
-    <t>stockholder's equity</t>
-  </si>
-  <si>
-    <t>shareholders equity</t>
-  </si>
-  <si>
     <t>total current assets</t>
   </si>
   <si>
@@ -341,51 +299,6 @@
   </si>
   <si>
     <t>other operating expenses</t>
-  </si>
-  <si>
-    <t>net cash flow from investing</t>
-  </si>
-  <si>
-    <t>net cash flow from investing activities</t>
-  </si>
-  <si>
-    <t>cash flow from financing</t>
-  </si>
-  <si>
-    <t>net cash flow from financing</t>
-  </si>
-  <si>
-    <t>cash flow from financing activities</t>
-  </si>
-  <si>
-    <t>net cash flow from financing activities</t>
-  </si>
-  <si>
-    <t>cash flow from investing activities</t>
-  </si>
-  <si>
-    <t>net increase in cash</t>
-  </si>
-  <si>
-    <t>closing cash balance</t>
-  </si>
-  <si>
-    <t>opening cash balance</t>
-  </si>
-  <si>
-    <t>cash paid for income taxes</t>
-  </si>
-  <si>
-    <t>cash paid for interest</t>
-  </si>
-  <si>
-    <t>cash beginning of period</t>
-  </si>
-  <si>
-    <t>cash end of period</t>
-  </si>
-  <si>
-    <t>net change in cash</t>
   </si>
 </sst>
 </file>
@@ -743,7 +656,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D25" sqref="C1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,413 +674,327 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
         <v>66</v>
       </c>
-      <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>